<commit_message>
Updated table of tools descriptions
</commit_message>
<xml_diff>
--- a/oxshef-viz-tools.xlsx
+++ b/oxshef-viz-tools.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29720" windowHeight="20080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34140" windowHeight="27380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>tool</t>
   </si>
@@ -80,17 +80,43 @@
 &lt;a href='http://oxshef-shiny.netlify.com' target='_blank' style='font-weight:bold'&gt;[Read more...]&lt;/a&gt;</t>
   </si>
   <si>
-    <t>A Grammar of Interactive Graphics built with JSON
-&lt;br&gt;
-&lt;a href='http://oxshef-vega-lite.netlify.com' target='_blank' style='font-weight:bold'&gt;[Read more...]&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Plotly provides a free tool for creating interactive visualisations from dataset uploaded to the Plotly service. It's a great tool for creating "one off" visualisations but does not fit into a fully reproducible workflow as data must be siloed in the plot.ly website.</t>
   </si>
   <si>
-    <t>Dash allows Python users to build rich interactive web applications and visualisations through a combination of different technologies, including React and Flask.
-&lt;br&gt;
-&lt;a href='http://oxshef-dash.netlify.com' target='_blank' style='font-weight:bold'&gt;[Read more...]&lt;/a&gt;</t>
+    <t>image.path</t>
+  </si>
+  <si>
+    <t>shiny-logo.png</t>
+  </si>
+  <si>
+    <t>plotly-logo.png</t>
+  </si>
+  <si>
+    <t>r-logo.png</t>
+  </si>
+  <si>
+    <t>dash-logo.svg</t>
+  </si>
+  <si>
+    <t>vega-lite-logo.png</t>
+  </si>
+  <si>
+    <t>Vega-Lite provides a high-level grammar of interactive graphics, allowing users to specify "charts as data" in well designed JSON format. OxShef are currently investigating the reproducability of a Vega-Lite driven dataviz workflow, which may lead to a dedicated site about this tool in the future.</t>
+  </si>
+  <si>
+    <t>Dash allows Python users to build rich interactive web applications and visualisations through a combination of different technologies, including React and Flask. OxShef are currently investigating the reproducability of a Dash-driven dataviz visualisation workflow, which may lead to a dedicated site about this tool in the future.</t>
+  </si>
+  <si>
+    <t>Jupyter</t>
+  </si>
+  <si>
+    <t>http://jupyter.org/</t>
+  </si>
+  <si>
+    <t>jupyter-logo.png</t>
+  </si>
+  <si>
+    <t>Jupyter (the spiritual successor to iPython notebooks) is a powerful tool for creating rich documents incorporating code, data and visualisation outputs. Jupyter notebooks allow code written in Python, R and more to be combined together easily. Oxshef are currently developing a site dedicated to using this tool in a reproducible dataviz workflow.</t>
   </si>
 </sst>
 </file>
@@ -427,120 +453,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="55.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="b">
+      <c r="F2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="b">
+      <c r="F3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="b">
+      <c r="F4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="137" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="137" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="b">
+      <c r="F5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="b">
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>